<commit_message>
got nparray on test file
</commit_message>
<xml_diff>
--- a/model/bank_statements/Llyods Bank.xlsx
+++ b/model/bank_statements/Llyods Bank.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>TFR Lloyds Bank - Print Friendly Statement</t>
-  </si>
-  <si>
-    <t>2469.06.</t>
   </si>
   <si>
     <t>LNK PO MITCHAM LAN CD 7420 11SEP15</t>
@@ -979,8 +976,8 @@
       <c r="E23" s="8">
         <v>10.5</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>33</v>
+      <c r="F23" s="5">
+        <v>2469.06</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
@@ -988,7 +985,7 @@
         <v>43762</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>7</v>
@@ -1006,7 +1003,7 @@
         <v>43765</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>11</v>
@@ -1024,7 +1021,7 @@
         <v>43768</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>11</v>
@@ -1042,7 +1039,7 @@
         <v>43774</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>11</v>
@@ -1060,7 +1057,7 @@
         <v>43775</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>11</v>
@@ -1078,7 +1075,7 @@
         <v>43776</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>16</v>
@@ -1096,7 +1093,7 @@
         <v>43780</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>7</v>
@@ -1114,7 +1111,7 @@
         <v>43782</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>11</v>
@@ -1150,10 +1147,10 @@
         <v>43783</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="D33" s="7">
         <v>870</v>
@@ -1168,7 +1165,7 @@
         <v>43786</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>11</v>
@@ -1186,7 +1183,7 @@
         <v>43787</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>7</v>
@@ -1204,7 +1201,7 @@
         <v>43788</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>11</v>
@@ -1222,7 +1219,7 @@
         <v>43788</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>9</v>
@@ -1240,7 +1237,7 @@
         <v>43791</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>11</v>

</xml_diff>